<commit_message>
main.py --> app.py added new excel sheet: annual_temp
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main Repo\Data-Science Projects\Climatology Philippines Choropleth Map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main Repo\Data-Science Projects\Philippines  - Climatology Choropleth Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5932B-3F30-47A2-A523-D908F8DC0A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78B3F5E-2E73-4497-80D3-5B8649D8FEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{947AB583-2011-409A-9F18-682A34E6FAE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{947AB583-2011-409A-9F18-682A34E6FAE7}"/>
   </bookViews>
   <sheets>
     <sheet name="max-temp" sheetId="1" r:id="rId1"/>
     <sheet name="min-temp" sheetId="2" r:id="rId2"/>
     <sheet name="mean-temp" sheetId="3" r:id="rId3"/>
+    <sheet name="annual_temp" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
   <si>
     <t>Annual</t>
   </si>
@@ -123,6 +124,18 @@
   </si>
   <si>
     <t>Metropolitan Manila (NCR)</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -2112,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685016A4-5955-4FBA-9A6D-692D47256CBF}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2917,4 +2930,1730 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E4EA49-8BB9-41EA-A3CC-957C454D1C20}">
+  <dimension ref="A1:D122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1901</v>
+      </c>
+      <c r="B2">
+        <v>25.79</v>
+      </c>
+      <c r="C2">
+        <v>21.31</v>
+      </c>
+      <c r="D2">
+        <v>30.31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1902</v>
+      </c>
+      <c r="B3">
+        <v>25.78</v>
+      </c>
+      <c r="C3">
+        <v>21.3</v>
+      </c>
+      <c r="D3">
+        <v>30.31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1903</v>
+      </c>
+      <c r="B4">
+        <v>25.45</v>
+      </c>
+      <c r="C4">
+        <v>21.15</v>
+      </c>
+      <c r="D4">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1904</v>
+      </c>
+      <c r="B5">
+        <v>24.83</v>
+      </c>
+      <c r="C5">
+        <v>20.52</v>
+      </c>
+      <c r="D5">
+        <v>29.19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1905</v>
+      </c>
+      <c r="B6">
+        <v>25.2</v>
+      </c>
+      <c r="C6">
+        <v>20.69</v>
+      </c>
+      <c r="D6">
+        <v>29.76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1906</v>
+      </c>
+      <c r="B7">
+        <v>25.48</v>
+      </c>
+      <c r="C7">
+        <v>20.99</v>
+      </c>
+      <c r="D7">
+        <v>30.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1907</v>
+      </c>
+      <c r="B8">
+        <v>25.15</v>
+      </c>
+      <c r="C8">
+        <v>20.64</v>
+      </c>
+      <c r="D8">
+        <v>29.71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1908</v>
+      </c>
+      <c r="B9">
+        <v>25.16</v>
+      </c>
+      <c r="C9">
+        <v>20.73</v>
+      </c>
+      <c r="D9">
+        <v>29.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1909</v>
+      </c>
+      <c r="B10">
+        <v>25.38</v>
+      </c>
+      <c r="C10">
+        <v>20.91</v>
+      </c>
+      <c r="D10">
+        <v>29.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1910</v>
+      </c>
+      <c r="B11">
+        <v>25.17</v>
+      </c>
+      <c r="C11">
+        <v>20.78</v>
+      </c>
+      <c r="D11">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1911</v>
+      </c>
+      <c r="B12">
+        <v>25.11</v>
+      </c>
+      <c r="C12">
+        <v>20.41</v>
+      </c>
+      <c r="D12">
+        <v>29.86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1912</v>
+      </c>
+      <c r="B13">
+        <v>25.47</v>
+      </c>
+      <c r="C13">
+        <v>20.66</v>
+      </c>
+      <c r="D13">
+        <v>30.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1913</v>
+      </c>
+      <c r="B14">
+        <v>25.25</v>
+      </c>
+      <c r="C14">
+        <v>20.65</v>
+      </c>
+      <c r="D14">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1914</v>
+      </c>
+      <c r="B15">
+        <v>25.47</v>
+      </c>
+      <c r="C15">
+        <v>20.88</v>
+      </c>
+      <c r="D15">
+        <v>30.11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1915</v>
+      </c>
+      <c r="B16">
+        <v>25.9</v>
+      </c>
+      <c r="C16">
+        <v>21.31</v>
+      </c>
+      <c r="D16">
+        <v>30.53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1916</v>
+      </c>
+      <c r="B17">
+        <v>25.26</v>
+      </c>
+      <c r="C17">
+        <v>20.93</v>
+      </c>
+      <c r="D17">
+        <v>29.64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1917</v>
+      </c>
+      <c r="B18">
+        <v>25.01</v>
+      </c>
+      <c r="C18">
+        <v>20.63</v>
+      </c>
+      <c r="D18">
+        <v>29.44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1918</v>
+      </c>
+      <c r="B19">
+        <v>24.89</v>
+      </c>
+      <c r="C19">
+        <v>20.56</v>
+      </c>
+      <c r="D19">
+        <v>29.26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1919</v>
+      </c>
+      <c r="B20">
+        <v>25.5</v>
+      </c>
+      <c r="C20">
+        <v>21.03</v>
+      </c>
+      <c r="D20">
+        <v>30.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1920</v>
+      </c>
+      <c r="B21">
+        <v>25.44</v>
+      </c>
+      <c r="C21">
+        <v>21.03</v>
+      </c>
+      <c r="D21">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1921</v>
+      </c>
+      <c r="B22">
+        <v>25.22</v>
+      </c>
+      <c r="C22">
+        <v>20.86</v>
+      </c>
+      <c r="D22">
+        <v>29.64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1922</v>
+      </c>
+      <c r="B23">
+        <v>25.47</v>
+      </c>
+      <c r="C23">
+        <v>21.09</v>
+      </c>
+      <c r="D23">
+        <v>29.89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1923</v>
+      </c>
+      <c r="B24">
+        <v>25.13</v>
+      </c>
+      <c r="C24">
+        <v>20.73</v>
+      </c>
+      <c r="D24">
+        <v>29.57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1924</v>
+      </c>
+      <c r="B25">
+        <v>25.43</v>
+      </c>
+      <c r="C25">
+        <v>21.12</v>
+      </c>
+      <c r="D25">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1925</v>
+      </c>
+      <c r="B26">
+        <v>25.23</v>
+      </c>
+      <c r="C26">
+        <v>21</v>
+      </c>
+      <c r="D26">
+        <v>29.51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1926</v>
+      </c>
+      <c r="B27">
+        <v>25.42</v>
+      </c>
+      <c r="C27">
+        <v>21.1</v>
+      </c>
+      <c r="D27">
+        <v>29.79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1927</v>
+      </c>
+      <c r="B28">
+        <v>25.54</v>
+      </c>
+      <c r="C28">
+        <v>21.19</v>
+      </c>
+      <c r="D28">
+        <v>29.94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1928</v>
+      </c>
+      <c r="B29">
+        <v>25.65</v>
+      </c>
+      <c r="C29">
+        <v>21.36</v>
+      </c>
+      <c r="D29">
+        <v>29.99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1929</v>
+      </c>
+      <c r="B30">
+        <v>25.24</v>
+      </c>
+      <c r="C30">
+        <v>20.9</v>
+      </c>
+      <c r="D30">
+        <v>29.62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1930</v>
+      </c>
+      <c r="B31">
+        <v>25.68</v>
+      </c>
+      <c r="C31">
+        <v>21.27</v>
+      </c>
+      <c r="D31">
+        <v>30.14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1931</v>
+      </c>
+      <c r="B32">
+        <v>26.02</v>
+      </c>
+      <c r="C32">
+        <v>21.63</v>
+      </c>
+      <c r="D32">
+        <v>30.46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1932</v>
+      </c>
+      <c r="B33">
+        <v>25.47</v>
+      </c>
+      <c r="C33">
+        <v>21.23</v>
+      </c>
+      <c r="D33">
+        <v>29.77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1933</v>
+      </c>
+      <c r="B34">
+        <v>25.69</v>
+      </c>
+      <c r="C34">
+        <v>21.43</v>
+      </c>
+      <c r="D34">
+        <v>29.99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1934</v>
+      </c>
+      <c r="B35">
+        <v>25.32</v>
+      </c>
+      <c r="C35">
+        <v>21.29</v>
+      </c>
+      <c r="D35">
+        <v>29.39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1935</v>
+      </c>
+      <c r="B36">
+        <v>25.61</v>
+      </c>
+      <c r="C36">
+        <v>21.35</v>
+      </c>
+      <c r="D36">
+        <v>29.93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1936</v>
+      </c>
+      <c r="B37">
+        <v>25.67</v>
+      </c>
+      <c r="C37">
+        <v>21.41</v>
+      </c>
+      <c r="D37">
+        <v>29.98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1937</v>
+      </c>
+      <c r="B38">
+        <v>25.82</v>
+      </c>
+      <c r="C38">
+        <v>21.41</v>
+      </c>
+      <c r="D38">
+        <v>30.28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1938</v>
+      </c>
+      <c r="B39">
+        <v>25.67</v>
+      </c>
+      <c r="C39">
+        <v>21.36</v>
+      </c>
+      <c r="D39">
+        <v>30.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1939</v>
+      </c>
+      <c r="B40">
+        <v>25.59</v>
+      </c>
+      <c r="C40">
+        <v>21.38</v>
+      </c>
+      <c r="D40">
+        <v>29.85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1940</v>
+      </c>
+      <c r="B41">
+        <v>25.63</v>
+      </c>
+      <c r="C41">
+        <v>21.16</v>
+      </c>
+      <c r="D41">
+        <v>30.14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1941</v>
+      </c>
+      <c r="B42">
+        <v>25.75</v>
+      </c>
+      <c r="C42">
+        <v>21.28</v>
+      </c>
+      <c r="D42">
+        <v>30.27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1942</v>
+      </c>
+      <c r="B43">
+        <v>25.68</v>
+      </c>
+      <c r="C43">
+        <v>21.2</v>
+      </c>
+      <c r="D43">
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1943</v>
+      </c>
+      <c r="B44">
+        <v>25.52</v>
+      </c>
+      <c r="C44">
+        <v>21.04</v>
+      </c>
+      <c r="D44">
+        <v>30.05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1944</v>
+      </c>
+      <c r="B45">
+        <v>25.6</v>
+      </c>
+      <c r="C45">
+        <v>21.12</v>
+      </c>
+      <c r="D45">
+        <v>30.13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1945</v>
+      </c>
+      <c r="B46">
+        <v>25.53</v>
+      </c>
+      <c r="C46">
+        <v>21.11</v>
+      </c>
+      <c r="D46">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1946</v>
+      </c>
+      <c r="B47">
+        <v>25.83</v>
+      </c>
+      <c r="C47">
+        <v>21.31</v>
+      </c>
+      <c r="D47">
+        <v>30.41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1947</v>
+      </c>
+      <c r="B48">
+        <v>26.07</v>
+      </c>
+      <c r="C48">
+        <v>21.64</v>
+      </c>
+      <c r="D48">
+        <v>30.55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1948</v>
+      </c>
+      <c r="B49">
+        <v>25.81</v>
+      </c>
+      <c r="C49">
+        <v>21.33</v>
+      </c>
+      <c r="D49">
+        <v>30.34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1949</v>
+      </c>
+      <c r="B50">
+        <v>25.46</v>
+      </c>
+      <c r="C50">
+        <v>21.05</v>
+      </c>
+      <c r="D50">
+        <v>29.92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1950</v>
+      </c>
+      <c r="B51">
+        <v>25.47</v>
+      </c>
+      <c r="C51">
+        <v>21.11</v>
+      </c>
+      <c r="D51">
+        <v>29.89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1951</v>
+      </c>
+      <c r="B52">
+        <v>25.63</v>
+      </c>
+      <c r="C52">
+        <v>21.14</v>
+      </c>
+      <c r="D52">
+        <v>30.17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1952</v>
+      </c>
+      <c r="B53">
+        <v>25.7</v>
+      </c>
+      <c r="C53">
+        <v>21.24</v>
+      </c>
+      <c r="D53">
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1953</v>
+      </c>
+      <c r="B54">
+        <v>25.67</v>
+      </c>
+      <c r="C54">
+        <v>21.22</v>
+      </c>
+      <c r="D54">
+        <v>30.18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1954</v>
+      </c>
+      <c r="B55">
+        <v>25.59</v>
+      </c>
+      <c r="C55">
+        <v>20.99</v>
+      </c>
+      <c r="D55">
+        <v>30.25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1955</v>
+      </c>
+      <c r="B56">
+        <v>25.36</v>
+      </c>
+      <c r="C56">
+        <v>20.89</v>
+      </c>
+      <c r="D56">
+        <v>29.89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1956</v>
+      </c>
+      <c r="B57">
+        <v>25.33</v>
+      </c>
+      <c r="C57">
+        <v>21.01</v>
+      </c>
+      <c r="D57">
+        <v>29.69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1957</v>
+      </c>
+      <c r="B58">
+        <v>25.66</v>
+      </c>
+      <c r="C58">
+        <v>21.19</v>
+      </c>
+      <c r="D58">
+        <v>30.18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1958</v>
+      </c>
+      <c r="B59">
+        <v>25.64</v>
+      </c>
+      <c r="C59">
+        <v>21.19</v>
+      </c>
+      <c r="D59">
+        <v>30.14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1959</v>
+      </c>
+      <c r="B60">
+        <v>25.62</v>
+      </c>
+      <c r="C60">
+        <v>21.12</v>
+      </c>
+      <c r="D60">
+        <v>30.17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1960</v>
+      </c>
+      <c r="B61">
+        <v>25.66</v>
+      </c>
+      <c r="C61">
+        <v>21.24</v>
+      </c>
+      <c r="D61">
+        <v>30.13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1961</v>
+      </c>
+      <c r="B62">
+        <v>25.5</v>
+      </c>
+      <c r="C62">
+        <v>21</v>
+      </c>
+      <c r="D62">
+        <v>30.06</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1962</v>
+      </c>
+      <c r="B63">
+        <v>25.4</v>
+      </c>
+      <c r="C63">
+        <v>20.94</v>
+      </c>
+      <c r="D63">
+        <v>29.91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1963</v>
+      </c>
+      <c r="B64">
+        <v>25.25</v>
+      </c>
+      <c r="C64">
+        <v>20.78</v>
+      </c>
+      <c r="D64">
+        <v>29.77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1964</v>
+      </c>
+      <c r="B65">
+        <v>25.56</v>
+      </c>
+      <c r="C65">
+        <v>21.15</v>
+      </c>
+      <c r="D65">
+        <v>30.01</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1965</v>
+      </c>
+      <c r="B66">
+        <v>25.38</v>
+      </c>
+      <c r="C66">
+        <v>20.98</v>
+      </c>
+      <c r="D66">
+        <v>29.82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1966</v>
+      </c>
+      <c r="B67">
+        <v>25.82</v>
+      </c>
+      <c r="C67">
+        <v>21.39</v>
+      </c>
+      <c r="D67">
+        <v>30.31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1967</v>
+      </c>
+      <c r="B68">
+        <v>25.28</v>
+      </c>
+      <c r="C68">
+        <v>20.89</v>
+      </c>
+      <c r="D68">
+        <v>29.72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1968</v>
+      </c>
+      <c r="B69">
+        <v>25.45</v>
+      </c>
+      <c r="C69">
+        <v>20.83</v>
+      </c>
+      <c r="D69">
+        <v>30.12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1969</v>
+      </c>
+      <c r="B70">
+        <v>25.76</v>
+      </c>
+      <c r="C70">
+        <v>21.14</v>
+      </c>
+      <c r="D70">
+        <v>30.43</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1970</v>
+      </c>
+      <c r="B71">
+        <v>25.86</v>
+      </c>
+      <c r="C71">
+        <v>21.43</v>
+      </c>
+      <c r="D71">
+        <v>30.34</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1971</v>
+      </c>
+      <c r="B72">
+        <v>25.21</v>
+      </c>
+      <c r="C72">
+        <v>20.79</v>
+      </c>
+      <c r="D72">
+        <v>29.68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1972</v>
+      </c>
+      <c r="B73">
+        <v>25.49</v>
+      </c>
+      <c r="C73">
+        <v>20.91</v>
+      </c>
+      <c r="D73">
+        <v>30.13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1973</v>
+      </c>
+      <c r="B74">
+        <v>25.8</v>
+      </c>
+      <c r="C74">
+        <v>21.21</v>
+      </c>
+      <c r="D74">
+        <v>30.45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1974</v>
+      </c>
+      <c r="B75">
+        <v>25.58</v>
+      </c>
+      <c r="C75">
+        <v>21.24</v>
+      </c>
+      <c r="D75">
+        <v>29.98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1975</v>
+      </c>
+      <c r="B76">
+        <v>25.53</v>
+      </c>
+      <c r="C76">
+        <v>21.11</v>
+      </c>
+      <c r="D76">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1976</v>
+      </c>
+      <c r="B77">
+        <v>25.36</v>
+      </c>
+      <c r="C77">
+        <v>20.99</v>
+      </c>
+      <c r="D77">
+        <v>29.78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1977</v>
+      </c>
+      <c r="B78">
+        <v>25.74</v>
+      </c>
+      <c r="C78">
+        <v>21.38</v>
+      </c>
+      <c r="D78">
+        <v>30.15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1978</v>
+      </c>
+      <c r="B79">
+        <v>25.72</v>
+      </c>
+      <c r="C79">
+        <v>21.34</v>
+      </c>
+      <c r="D79">
+        <v>30.15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1979</v>
+      </c>
+      <c r="B80">
+        <v>25.85</v>
+      </c>
+      <c r="C80">
+        <v>21.32</v>
+      </c>
+      <c r="D80">
+        <v>30.44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1980</v>
+      </c>
+      <c r="B81">
+        <v>25.92</v>
+      </c>
+      <c r="C81">
+        <v>21.57</v>
+      </c>
+      <c r="D81">
+        <v>30.32</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1981</v>
+      </c>
+      <c r="B82">
+        <v>25.54</v>
+      </c>
+      <c r="C82">
+        <v>21.07</v>
+      </c>
+      <c r="D82">
+        <v>30.06</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1982</v>
+      </c>
+      <c r="B83">
+        <v>25.66</v>
+      </c>
+      <c r="C83">
+        <v>21.15</v>
+      </c>
+      <c r="D83">
+        <v>30.22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1983</v>
+      </c>
+      <c r="B84">
+        <v>26.05</v>
+      </c>
+      <c r="C84">
+        <v>21.43</v>
+      </c>
+      <c r="D84">
+        <v>30.72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1984</v>
+      </c>
+      <c r="B85">
+        <v>25.81</v>
+      </c>
+      <c r="C85">
+        <v>21.38</v>
+      </c>
+      <c r="D85">
+        <v>30.28</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>1985</v>
+      </c>
+      <c r="B86">
+        <v>25.91</v>
+      </c>
+      <c r="C86">
+        <v>21.42</v>
+      </c>
+      <c r="D86">
+        <v>30.45</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>1986</v>
+      </c>
+      <c r="B87">
+        <v>25.81</v>
+      </c>
+      <c r="C87">
+        <v>21.35</v>
+      </c>
+      <c r="D87">
+        <v>30.32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>1987</v>
+      </c>
+      <c r="B88">
+        <v>26.32</v>
+      </c>
+      <c r="C88">
+        <v>21.64</v>
+      </c>
+      <c r="D88">
+        <v>31.06</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1988</v>
+      </c>
+      <c r="B89">
+        <v>26.27</v>
+      </c>
+      <c r="C89">
+        <v>21.72</v>
+      </c>
+      <c r="D89">
+        <v>30.86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>1989</v>
+      </c>
+      <c r="B90">
+        <v>25.82</v>
+      </c>
+      <c r="C90">
+        <v>21.32</v>
+      </c>
+      <c r="D90">
+        <v>30.38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1990</v>
+      </c>
+      <c r="B91">
+        <v>26.08</v>
+      </c>
+      <c r="C91">
+        <v>21.56</v>
+      </c>
+      <c r="D91">
+        <v>30.66</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1991</v>
+      </c>
+      <c r="B92">
+        <v>26.07</v>
+      </c>
+      <c r="C92">
+        <v>21.6</v>
+      </c>
+      <c r="D92">
+        <v>30.59</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1992</v>
+      </c>
+      <c r="B93">
+        <v>25.91</v>
+      </c>
+      <c r="C93">
+        <v>21.23</v>
+      </c>
+      <c r="D93">
+        <v>30.64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1993</v>
+      </c>
+      <c r="B94">
+        <v>26.02</v>
+      </c>
+      <c r="C94">
+        <v>21.55</v>
+      </c>
+      <c r="D94">
+        <v>30.53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1994</v>
+      </c>
+      <c r="B95">
+        <v>26.14</v>
+      </c>
+      <c r="C95">
+        <v>21.73</v>
+      </c>
+      <c r="D95">
+        <v>30.59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>1995</v>
+      </c>
+      <c r="B96">
+        <v>26.01</v>
+      </c>
+      <c r="C96">
+        <v>21.71</v>
+      </c>
+      <c r="D96">
+        <v>30.35</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1996</v>
+      </c>
+      <c r="B97">
+        <v>25.88</v>
+      </c>
+      <c r="C97">
+        <v>21.78</v>
+      </c>
+      <c r="D97">
+        <v>30.03</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1997</v>
+      </c>
+      <c r="B98">
+        <v>25.97</v>
+      </c>
+      <c r="C98">
+        <v>21.64</v>
+      </c>
+      <c r="D98">
+        <v>30.36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>1998</v>
+      </c>
+      <c r="B99">
+        <v>26.65</v>
+      </c>
+      <c r="C99">
+        <v>22.25</v>
+      </c>
+      <c r="D99">
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1999</v>
+      </c>
+      <c r="B100">
+        <v>26</v>
+      </c>
+      <c r="C100">
+        <v>21.93</v>
+      </c>
+      <c r="D100">
+        <v>30.12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2000</v>
+      </c>
+      <c r="B101">
+        <v>26.13</v>
+      </c>
+      <c r="C101">
+        <v>22.08</v>
+      </c>
+      <c r="D101">
+        <v>30.24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2001</v>
+      </c>
+      <c r="B102">
+        <v>26.19</v>
+      </c>
+      <c r="C102">
+        <v>21.99</v>
+      </c>
+      <c r="D102">
+        <v>30.43</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>2002</v>
+      </c>
+      <c r="B103">
+        <v>26.07</v>
+      </c>
+      <c r="C103">
+        <v>21.79</v>
+      </c>
+      <c r="D103">
+        <v>30.4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2003</v>
+      </c>
+      <c r="B104">
+        <v>25.95</v>
+      </c>
+      <c r="C104">
+        <v>21.57</v>
+      </c>
+      <c r="D104">
+        <v>30.38</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>2004</v>
+      </c>
+      <c r="B105">
+        <v>26.04</v>
+      </c>
+      <c r="C105">
+        <v>21.72</v>
+      </c>
+      <c r="D105">
+        <v>30.41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2005</v>
+      </c>
+      <c r="B106">
+        <v>26.14</v>
+      </c>
+      <c r="C106">
+        <v>21.87</v>
+      </c>
+      <c r="D106">
+        <v>30.47</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>2006</v>
+      </c>
+      <c r="B107">
+        <v>26.2</v>
+      </c>
+      <c r="C107">
+        <v>21.95</v>
+      </c>
+      <c r="D107">
+        <v>30.49</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2007</v>
+      </c>
+      <c r="B108">
+        <v>26.19</v>
+      </c>
+      <c r="C108">
+        <v>22.08</v>
+      </c>
+      <c r="D108">
+        <v>30.36</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2008</v>
+      </c>
+      <c r="B109">
+        <v>25.87</v>
+      </c>
+      <c r="C109">
+        <v>21.75</v>
+      </c>
+      <c r="D109">
+        <v>30.03</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>2009</v>
+      </c>
+      <c r="B110">
+        <v>25.9</v>
+      </c>
+      <c r="C110">
+        <v>21.74</v>
+      </c>
+      <c r="D110">
+        <v>30.11</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2010</v>
+      </c>
+      <c r="B111">
+        <v>26.17</v>
+      </c>
+      <c r="C111">
+        <v>21.88</v>
+      </c>
+      <c r="D111">
+        <v>30.51</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>2011</v>
+      </c>
+      <c r="B112">
+        <v>25.93</v>
+      </c>
+      <c r="C112">
+        <v>21.8</v>
+      </c>
+      <c r="D112">
+        <v>30.11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>2012</v>
+      </c>
+      <c r="B113">
+        <v>26.27</v>
+      </c>
+      <c r="C113">
+        <v>22.07</v>
+      </c>
+      <c r="D113">
+        <v>30.53</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>2013</v>
+      </c>
+      <c r="B114">
+        <v>26.28</v>
+      </c>
+      <c r="C114">
+        <v>22.06</v>
+      </c>
+      <c r="D114">
+        <v>30.55</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>2014</v>
+      </c>
+      <c r="B115">
+        <v>26.15</v>
+      </c>
+      <c r="C115">
+        <v>21.89</v>
+      </c>
+      <c r="D115">
+        <v>30.46</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2015</v>
+      </c>
+      <c r="B116">
+        <v>26.36</v>
+      </c>
+      <c r="C116">
+        <v>22.08</v>
+      </c>
+      <c r="D116">
+        <v>30.7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>2016</v>
+      </c>
+      <c r="B117">
+        <v>26.7</v>
+      </c>
+      <c r="C117">
+        <v>22.57</v>
+      </c>
+      <c r="D117">
+        <v>30.88</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>2017</v>
+      </c>
+      <c r="B118">
+        <v>26.26</v>
+      </c>
+      <c r="C118">
+        <v>22.21</v>
+      </c>
+      <c r="D118">
+        <v>30.35</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>2018</v>
+      </c>
+      <c r="B119">
+        <v>26.45</v>
+      </c>
+      <c r="C119">
+        <v>22.26</v>
+      </c>
+      <c r="D119">
+        <v>30.69</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>2019</v>
+      </c>
+      <c r="B120">
+        <v>26.52</v>
+      </c>
+      <c r="C120">
+        <v>22.39</v>
+      </c>
+      <c r="D120">
+        <v>30.71</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>2020</v>
+      </c>
+      <c r="B121">
+        <v>26.64</v>
+      </c>
+      <c r="C121">
+        <v>22.51</v>
+      </c>
+      <c r="D121">
+        <v>30.82</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>2021</v>
+      </c>
+      <c r="B122">
+        <v>26.6</v>
+      </c>
+      <c r="C122">
+        <v>22.52</v>
+      </c>
+      <c r="D122">
+        <v>30.74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modified: app.py, data.xlsx, lineGraph.py, staticMap.py
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main Repo\Data-Science Projects\Philippines  - Climatology Choropleth Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78B3F5E-2E73-4497-80D3-5B8649D8FEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75795E39-C2E6-4543-A734-16BF637EC942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{947AB583-2011-409A-9F18-682A34E6FAE7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{947AB583-2011-409A-9F18-682A34E6FAE7}"/>
   </bookViews>
   <sheets>
     <sheet name="max-temp" sheetId="1" r:id="rId1"/>
     <sheet name="min-temp" sheetId="2" r:id="rId2"/>
     <sheet name="mean-temp" sheetId="3" r:id="rId3"/>
     <sheet name="annual_temp" sheetId="4" r:id="rId4"/>
+    <sheet name="monthly_ph" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
   <si>
     <t>Annual</t>
   </si>
@@ -136,6 +137,12 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>precipitation</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -2936,7 +2943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E4EA49-8BB9-41EA-A3CC-957C454D1C20}">
   <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -4656,4 +4663,242 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928C9BCA-EC08-4B45-8687-F8E8DBECF185}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>20.86</v>
+      </c>
+      <c r="C2">
+        <v>24.96</v>
+      </c>
+      <c r="D2">
+        <v>29.11</v>
+      </c>
+      <c r="E2">
+        <v>160.82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>20.83</v>
+      </c>
+      <c r="C3">
+        <v>25.18</v>
+      </c>
+      <c r="D3">
+        <v>29.59</v>
+      </c>
+      <c r="E3">
+        <v>118.73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>21.42</v>
+      </c>
+      <c r="C4">
+        <v>26.09</v>
+      </c>
+      <c r="D4">
+        <v>30.81</v>
+      </c>
+      <c r="E4">
+        <v>117.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>22.33</v>
+      </c>
+      <c r="C5">
+        <v>27.09</v>
+      </c>
+      <c r="D5">
+        <v>31.89</v>
+      </c>
+      <c r="E5">
+        <v>116.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>22.87</v>
+      </c>
+      <c r="C6">
+        <v>27.42</v>
+      </c>
+      <c r="D6">
+        <v>32.020000000000003</v>
+      </c>
+      <c r="E6">
+        <v>203.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>22.59</v>
+      </c>
+      <c r="C7">
+        <v>26.85</v>
+      </c>
+      <c r="D7">
+        <v>31.16</v>
+      </c>
+      <c r="E7">
+        <v>251.66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>22.27</v>
+      </c>
+      <c r="C8">
+        <v>26.31</v>
+      </c>
+      <c r="D8">
+        <v>30.4</v>
+      </c>
+      <c r="E8">
+        <v>290.62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>22.3</v>
+      </c>
+      <c r="C9">
+        <v>26.28</v>
+      </c>
+      <c r="D9">
+        <v>30.31</v>
+      </c>
+      <c r="E9">
+        <v>314.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>22.18</v>
+      </c>
+      <c r="C10">
+        <v>26.26</v>
+      </c>
+      <c r="D10">
+        <v>30.38</v>
+      </c>
+      <c r="E10">
+        <v>276.13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>22.01</v>
+      </c>
+      <c r="C11">
+        <v>26.17</v>
+      </c>
+      <c r="D11">
+        <v>30.39</v>
+      </c>
+      <c r="E11">
+        <v>280.33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>21.87</v>
+      </c>
+      <c r="C12">
+        <v>25.95</v>
+      </c>
+      <c r="D12">
+        <v>30.07</v>
+      </c>
+      <c r="E12">
+        <v>251.71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>21.49</v>
+      </c>
+      <c r="C13">
+        <v>25.43</v>
+      </c>
+      <c r="D13">
+        <v>29.42</v>
+      </c>
+      <c r="E13">
+        <v>254.52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>